<commit_message>
Updated beneficial vs non-beneficial
Updated parameter definitions based on discussion in 6/14 meeting.
</commit_message>
<xml_diff>
--- a/criteria_weight_scenarios.xlsx
+++ b/criteria_weight_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlohm\Dropbox\Lohman-Guest_Shared\12_PhD_Paper3_Sanitation_Decision-Making\Python Code\GitHubDesktop\DMsan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34889F5-8EF2-415B-A38C-F30F10E55781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D72D1A1-A376-4640-B671-D8267D230EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E854125C-2344-44F6-A254-41B8AFA7B554}"/>
+    <workbookView xWindow="27210" yWindow="1425" windowWidth="19140" windowHeight="10200" xr2:uid="{E854125C-2344-44F6-A254-41B8AFA7B554}"/>
   </bookViews>
   <sheets>
     <sheet name="definitions" sheetId="4" r:id="rId1"/>
@@ -311,9 +311,6 @@
     <t>Impact of storms</t>
   </si>
   <si>
-    <t>Impact of extreme temperature changes</t>
-  </si>
-  <si>
     <t>Impact of droughts</t>
   </si>
   <si>
@@ -384,6 +381,9 @@
   </si>
   <si>
     <t>Weight_11</t>
+  </si>
+  <si>
+    <t>Impact power outages</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -507,18 +507,20 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -833,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DAC3413-5145-4E90-ADD4-96F1E182146D}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -848,7 +850,7 @@
     <col min="6" max="7" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -871,7 +873,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -895,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -919,7 +921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -943,7 +945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -967,7 +969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -991,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1015,103 +1017,105 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="D10" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="D11" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F11" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>44</v>
       </c>
@@ -1135,7 +1139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>44</v>
       </c>
@@ -1159,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>44</v>
       </c>
@@ -1183,7 +1187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>44</v>
       </c>
@@ -1207,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>44</v>
       </c>
@@ -1231,7 +1235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>44</v>
       </c>
@@ -1255,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>5</v>
       </c>
@@ -1271,15 +1275,16 @@
       <c r="E18" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G18" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>5</v>
       </c>
@@ -1295,15 +1300,16 @@
       <c r="E19" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>5</v>
       </c>
@@ -1319,328 +1325,331 @@
       <c r="E20" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
+      <c r="G20" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
+      <c r="G21" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="10" t="s">
+      <c r="B22" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="10" t="s">
+      <c r="E23" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="B24" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
+      <c r="E24" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="B25" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D25" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="10" t="s">
+      <c r="E25" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C25" s="10" t="s">
+      <c r="B26" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D26" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
+      <c r="E26" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="10" t="s">
+      <c r="B27" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D27" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
+      <c r="E27" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="10" t="s">
+      <c r="B28" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D28" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
+      <c r="E28" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="10" t="s">
+      <c r="B29" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D29" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="10" t="s">
+      <c r="E29" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="10" t="s">
+      <c r="B30" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D30" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
+      <c r="E30" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="10" t="s">
+      <c r="B31" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="10" t="s">
+      <c r="E31" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D31" s="10" t="s">
+      <c r="B32" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E31" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="10" t="s">
+      <c r="E32" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D32" s="10" t="s">
+      <c r="B33" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F33" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F33" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D34" s="1"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D35" s="1"/>
@@ -1662,7 +1671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6956783-CD8A-4021-B812-DCE07115A14C}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -1698,22 +1707,22 @@
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="14">
-        <v>1</v>
-      </c>
-      <c r="D2" s="14">
-        <v>0</v>
-      </c>
-      <c r="E2" s="14">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14">
-        <v>0</v>
-      </c>
-      <c r="G2" s="14">
+      <c r="B2" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0</v>
+      </c>
+      <c r="G2" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1721,22 +1730,22 @@
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="14">
-        <v>0</v>
-      </c>
-      <c r="D3" s="14">
-        <v>1</v>
-      </c>
-      <c r="E3" s="14">
-        <v>0</v>
-      </c>
-      <c r="F3" s="14">
-        <v>0</v>
-      </c>
-      <c r="G3" s="15">
+      <c r="B3" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+      <c r="G3" s="12">
         <v>0</v>
       </c>
     </row>
@@ -1744,22 +1753,22 @@
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="14">
-        <v>0</v>
-      </c>
-      <c r="D4" s="14">
-        <v>0</v>
-      </c>
-      <c r="E4" s="14">
-        <v>1</v>
-      </c>
-      <c r="F4" s="15">
-        <v>0</v>
-      </c>
-      <c r="G4" s="15">
+      <c r="B4" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12">
         <v>0</v>
       </c>
     </row>
@@ -1767,22 +1776,22 @@
       <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" s="15">
-        <v>0</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0</v>
-      </c>
-      <c r="E5" s="14">
-        <v>0</v>
-      </c>
-      <c r="F5" s="14">
-        <v>1</v>
-      </c>
-      <c r="G5" s="15">
+      <c r="B5" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12">
         <v>0</v>
       </c>
     </row>
@@ -1790,22 +1799,22 @@
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="15">
-        <v>0</v>
-      </c>
-      <c r="D6" s="14">
-        <v>0</v>
-      </c>
-      <c r="E6" s="14">
-        <v>0</v>
-      </c>
-      <c r="F6" s="15">
-        <v>0</v>
-      </c>
-      <c r="G6" s="14">
+      <c r="B6" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+      <c r="G6" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1834,7 +1843,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
@@ -1857,7 +1866,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -1880,7 +1889,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
@@ -1903,7 +1912,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
@@ -1926,7 +1935,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
@@ -1958,106 +1967,106 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="U1" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="W1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="X1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Y1" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="Z1" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AA1" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AB1" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AC1" s="13" t="s">
+      <c r="AC1" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="AD1" s="13" t="s">
+      <c r="AD1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="AE1" s="13" t="s">
+      <c r="AE1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="AF1" s="13" t="s">
+      <c r="AF1" s="10" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2159,134 +2168,102 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A3" s="12">
-        <f t="shared" ref="A3:AF3" si="0">IF(A2="beneficial", 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="B3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="X3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Y3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Z3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AB3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AC3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AF3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="3" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17">
+        <v>1</v>
+      </c>
+      <c r="C3" s="17">
+        <v>1</v>
+      </c>
+      <c r="D3" s="17">
+        <v>1</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1</v>
+      </c>
+      <c r="F3" s="17">
+        <v>1</v>
+      </c>
+      <c r="G3" s="17">
+        <v>1</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0</v>
+      </c>
+      <c r="I3" s="17">
+        <v>1</v>
+      </c>
+      <c r="J3" s="17">
+        <v>1</v>
+      </c>
+      <c r="K3" s="17">
+        <v>1</v>
+      </c>
+      <c r="L3" s="17">
+        <v>1</v>
+      </c>
+      <c r="M3" s="17">
+        <v>1</v>
+      </c>
+      <c r="N3" s="17">
+        <v>1</v>
+      </c>
+      <c r="O3" s="17">
+        <v>1</v>
+      </c>
+      <c r="P3" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="17">
+        <v>0</v>
+      </c>
+      <c r="R3" s="17">
+        <v>0</v>
+      </c>
+      <c r="S3" s="17">
+        <v>0</v>
+      </c>
+      <c r="T3" s="17">
+        <v>0</v>
+      </c>
+      <c r="U3" s="17">
+        <v>1</v>
+      </c>
+      <c r="V3" s="17">
+        <v>1</v>
+      </c>
+      <c r="W3" s="17">
+        <v>1</v>
+      </c>
+      <c r="X3" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="17">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="17">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="17">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="17">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>